<commit_message>
Parcial II: PRograma Parcial
Subo programa con parcial, punto 2 parece que ya, falta verificar punto 1
</commit_message>
<xml_diff>
--- a/Excels/Ecuaciones-RungeKutta.xlsx
+++ b/Excels/Ecuaciones-RungeKutta.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Felipe's\Documents\GitHub\MetodosNumericos\Excels\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fabian\Documents\GitHub\MetodosNumericos\Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="x" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>x0</t>
   </si>
@@ -70,12 +70,18 @@
   </si>
   <si>
     <t>k4</t>
+  </si>
+  <si>
+    <t>tiempo</t>
+  </si>
+  <si>
+    <t>temp/concentra</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -180,7 +186,13 @@
       <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="2" name="CuadroTexto 1"/>
+            <xdr:cNvPr id="2" name="CuadroTexto 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
             <xdr:cNvSpPr txBox="1"/>
           </xdr:nvSpPr>
           <xdr:spPr>
@@ -328,7 +340,13 @@
       <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="3" name="CuadroTexto 2"/>
+            <xdr:cNvPr id="3" name="CuadroTexto 2">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
             <xdr:cNvSpPr txBox="1"/>
           </xdr:nvSpPr>
           <xdr:spPr>
@@ -463,7 +481,13 @@
       <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="4" name="CuadroTexto 3"/>
+            <xdr:cNvPr id="4" name="CuadroTexto 3">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
             <xdr:cNvSpPr txBox="1"/>
           </xdr:nvSpPr>
           <xdr:spPr>
@@ -851,11 +875,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1096,6 +1120,17 @@
         <v>12.5</v>
       </c>
     </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E14" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14" t="s">
+        <v>16</v>
+      </c>
+      <c r="K14" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="E6:K6"/>
@@ -1107,7 +1142,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>